<commit_message>
Update product information ensuring customers see latest options and details
Refresh product database by replacing outdated data with current spreadsheet.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 0646a5b4-ba54-4146-8119-cc31c948a5ea
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/873c23c0-c18f-4e09-9f8d-38c5cb319996/02ac48d9-384e-4bbf-a986-9f451a3b5e80.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/Product Data_05_15_2025.xlsx
+++ b/attached_assets/Product Data_05_15_2025.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="315" documentId="11_BCFEBD4F73F15EB6C55EF89F1835901893D73E67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{464C7ED0-8AB6-4952-A9E5-BE29C579F396}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-2640" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shower Bases" sheetId="1" r:id="rId1"/>
@@ -5789,7 +5789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -31389,8 +31389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>